<commit_message>
Fix results excel file
</commit_message>
<xml_diff>
--- a/results/aggregated.xlsx
+++ b/results/aggregated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lin/Downloads/teapot-artifact 2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EA0509-7B88-5544-BD51-83710A63FF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA8508F-6E81-F641-914F-A421E4D77F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="8060" windowWidth="28100" windowHeight="17360" activeTab="1" xr2:uid="{924252C7-27FB-E746-A00E-47D3023788D1}"/>
+    <workbookView xWindow="6260" yWindow="3840" windowWidth="28100" windowHeight="17360" xr2:uid="{924252C7-27FB-E746-A00E-47D3023788D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Runtime Figure" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -525,28 +525,85 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -567,94 +624,31 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2031,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A727B6-291C-7E4C-8244-DC68B48EE29C}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D10"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2043,26 +2037,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="F1" s="23" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="F1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" ht="17" thickBot="1">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="17" thickTop="1">
       <c r="A3" s="1" t="s">
@@ -2091,19 +2085,19 @@
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
       <c r="F4" s="7" t="str">
         <f>A4</f>
         <v>brotli</v>
       </c>
-      <c r="G4" s="11" t="e">
-        <f>C4/$B$4</f>
+      <c r="G4" s="37" t="e">
+        <f>C4/$B4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H4" s="12" t="e">
-        <f>D4/$B$4</f>
+      <c r="H4" s="11" t="e">
+        <f>D4/$B4</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2111,18 +2105,18 @@
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
       <c r="F5" s="7" t="str">
         <f t="shared" ref="F5:F8" si="0">A5</f>
         <v>jsmn</v>
       </c>
-      <c r="G5" s="11" t="e">
-        <f t="shared" ref="G5:H8" si="1">C5/$B$4</f>
+      <c r="G5" s="37" t="e">
+        <f t="shared" ref="G5:H8" si="1">C5/$B5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H5" s="12" t="e">
+      <c r="H5" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -2131,18 +2125,18 @@
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
       <c r="F6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>libhtp</v>
       </c>
-      <c r="G6" s="11" t="e">
+      <c r="G6" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H6" s="12" t="e">
+      <c r="H6" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -2151,18 +2145,18 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
       <c r="F7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>openssl</v>
       </c>
-      <c r="G7" s="11" t="e">
+      <c r="G7" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H7" s="12" t="e">
+      <c r="H7" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -2171,35 +2165,35 @@
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
       <c r="F8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>yaml</v>
       </c>
-      <c r="G8" s="13" t="e">
+      <c r="G8" s="12" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="14" t="e">
+      <c r="H8" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" thickTop="1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2217,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B67C5B-4AFF-2D45-8842-1681C3F062E3}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2229,244 +2223,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" ht="17" thickBot="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" thickTop="1">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="23">
         <v>17</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="23">
         <v>68</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="36">
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="23">
         <f>SUM(E3:G3)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="36">
+      <c r="L3" s="23">
         <f>SUM(H3:J3)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="40">
+      <c r="M3" s="27">
         <f>SUM(K3:L3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="28">
         <v>1</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="28">
         <v>18</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="41">
+      <c r="D4" s="29"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="28">
         <f t="shared" ref="K4:K7" si="0">SUM(E4:G4)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="28">
         <f t="shared" ref="L4:L7" si="1">SUM(H4:J4)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="31">
         <f t="shared" ref="M4:M7" si="2">SUM(K4:L4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="28">
         <v>14</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="28">
         <v>91</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="41">
+      <c r="D5" s="29"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M5" s="44">
+      <c r="M5" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="28">
         <v>16</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="28">
         <v>589</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="41">
+      <c r="D6" s="29"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M6" s="44">
+      <c r="M6" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" thickBot="1">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="32">
         <v>3</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="32">
         <v>140</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="46">
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L7" s="46">
+      <c r="L7" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M7" s="50">
+      <c r="M7" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17" thickTop="1">
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="53" t="s">
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="D8:G9"/>
+    <mergeCell ref="H8:J9"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:M1"/>
-    <mergeCell ref="D8:G9"/>
-    <mergeCell ref="H8:J9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>